<commit_message>
Admin Unit packing upadted
</commit_message>
<xml_diff>
--- a/Excel/JibeAutomation.xlsx
+++ b/Excel/JibeAutomation.xlsx
@@ -19841,7 +19841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2053"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="C94" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -49744,8 +49744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>